<commit_message>
Change config-editor excel file
</commit_message>
<xml_diff>
--- a/schemas/dcat-ap/config-editor-fields.xlsx
+++ b/schemas/dcat-ap/config-editor-fields.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="101">
   <si>
     <t>Context</t>
   </si>
@@ -317,6 +317,9 @@
   </si>
   <si>
     <t>ok, maar in het nederlands is er maar 1 type en wordt dan dus niet goed getoond</t>
+  </si>
+  <si>
+    <t>dfqfds</t>
   </si>
 </sst>
 </file>
@@ -2992,10 +2995,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O27"/>
+  <dimension ref="A1:O28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4064,6 +4067,11 @@
     <row r="27" spans="1:15" x14ac:dyDescent="0.25">
       <c r="C27" t="s">
         <v>51</v>
+      </c>
+    </row>
+    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>100</v>
       </c>
     </row>
   </sheetData>

</xml_diff>